<commit_message>
added tests on fisheriris dataset
</commit_message>
<xml_diff>
--- a/Leg_Data_collect/Functions/Accuracy Results.xlsx
+++ b/Leg_Data_collect/Functions/Accuracy Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mural\Documents\GitHub\LegBot\Leg_Data_collect\Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10B1FDEC-98D9-4D20-B0E4-AEF4AA9F6833}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9579E224-D664-401E-98C1-3C64CEEC8270}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{91158D54-4C3B-48EB-A3A3-A69C65F9DEFF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>All Features</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>IrisData</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828ECD43-F68D-4E5B-8C9C-D02B65989447}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +411,7 @@
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +436,14 @@
       <c r="K1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>89</v>
       </c>
@@ -463,8 +472,15 @@
         <f>SUM(J2:J11)/10</f>
         <v>80.400000000000006</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>97.33</v>
+      </c>
+      <c r="N2">
+        <f>SUM(M2:M11)/10</f>
+        <v>95.199000000000026</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>76</v>
       </c>
@@ -477,8 +493,11 @@
       <c r="J3">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>94.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>86</v>
       </c>
@@ -491,8 +510,11 @@
       <c r="J4">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>85</v>
       </c>
@@ -505,8 +527,11 @@
       <c r="J5">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>94.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>78</v>
       </c>
@@ -519,8 +544,11 @@
       <c r="J6">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>85</v>
       </c>
@@ -533,8 +561,11 @@
       <c r="J7">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>83</v>
       </c>
@@ -547,8 +578,11 @@
       <c r="J8">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>93.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>83</v>
       </c>
@@ -561,8 +595,11 @@
       <c r="J9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>93.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>87</v>
       </c>
@@ -575,8 +612,11 @@
       <c r="J10">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>97.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>85</v>
       </c>
@@ -588,6 +628,9 @@
       </c>
       <c r="J11">
         <v>84</v>
+      </c>
+      <c r="M11">
+        <v>97.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>